<commit_message>
fixed bipartite graph and clusters
</commit_message>
<xml_diff>
--- a/currently_in_use/tests/Test_results.xlsx
+++ b/currently_in_use/tests/Test_results.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -680,6 +680,347 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2021-04-01 15:14:42.328650</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>11</v>
+      </c>
+      <c r="I8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>100</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2021-04-01 15:27:37.709801</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>34</v>
+      </c>
+      <c r="E9" t="n">
+        <v>34</v>
+      </c>
+      <c r="F9" t="n">
+        <v>32</v>
+      </c>
+      <c r="G9" t="n">
+        <v>34</v>
+      </c>
+      <c r="H9" t="n">
+        <v>34</v>
+      </c>
+      <c r="I9" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>100</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2021-04-01 15:28:44.328220</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E10" t="n">
+        <v>42</v>
+      </c>
+      <c r="F10" t="n">
+        <v>42</v>
+      </c>
+      <c r="G10" t="n">
+        <v>32</v>
+      </c>
+      <c r="H10" t="n">
+        <v>42</v>
+      </c>
+      <c r="I10" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>100</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2021-04-01 15:28:55.951325</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>37</v>
+      </c>
+      <c r="E11" t="n">
+        <v>36</v>
+      </c>
+      <c r="F11" t="n">
+        <v>37</v>
+      </c>
+      <c r="G11" t="n">
+        <v>36</v>
+      </c>
+      <c r="H11" t="n">
+        <v>37</v>
+      </c>
+      <c r="I11" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>100</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2021-04-01 15:29:05.953316</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>27</v>
+      </c>
+      <c r="E12" t="n">
+        <v>26</v>
+      </c>
+      <c r="F12" t="n">
+        <v>27</v>
+      </c>
+      <c r="G12" t="n">
+        <v>22</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27</v>
+      </c>
+      <c r="I12" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>50</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:28:10.365738</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" t="n">
+        <v>11</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>50</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:30:09.387693</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>30</v>
+      </c>
+      <c r="E14" t="n">
+        <v>30</v>
+      </c>
+      <c r="F14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>30</v>
+      </c>
+      <c r="I14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>50</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:30:20.690811</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>17</v>
+      </c>
+      <c r="E15" t="n">
+        <v>18</v>
+      </c>
+      <c r="F15" t="n">
+        <v>17</v>
+      </c>
+      <c r="G15" t="n">
+        <v>18</v>
+      </c>
+      <c r="H15" t="n">
+        <v>18</v>
+      </c>
+      <c r="I15" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>100</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:31:25.854300</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>45</v>
+      </c>
+      <c r="E16" t="n">
+        <v>43</v>
+      </c>
+      <c r="F16" t="n">
+        <v>46</v>
+      </c>
+      <c r="G16" t="n">
+        <v>18</v>
+      </c>
+      <c r="H16" t="n">
+        <v>46</v>
+      </c>
+      <c r="I16" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>100</v>
+      </c>
+      <c r="B17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:32:02.904430</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>46</v>
+      </c>
+      <c r="E17" t="n">
+        <v>47</v>
+      </c>
+      <c r="F17" t="n">
+        <v>47</v>
+      </c>
+      <c r="G17" t="n">
+        <v>33</v>
+      </c>
+      <c r="H17" t="n">
+        <v>47</v>
+      </c>
+      <c r="I17" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>100</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2021-04-08 10:33:05.418990</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>47</v>
+      </c>
+      <c r="E18" t="n">
+        <v>48</v>
+      </c>
+      <c r="F18" t="n">
+        <v>48</v>
+      </c>
+      <c r="G18" t="n">
+        <v>47</v>
+      </c>
+      <c r="H18" t="n">
+        <v>48</v>
+      </c>
+      <c r="I18" t="n">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added lots of comments
</commit_message>
<xml_diff>
--- a/currently_in_use/tests/Test_results.xlsx
+++ b/currently_in_use/tests/Test_results.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -1021,6 +1021,316 @@
         <v>48</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>100</v>
+      </c>
+      <c r="B19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:29:13.116392</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>11</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9</v>
+      </c>
+      <c r="F19" t="n">
+        <v>9</v>
+      </c>
+      <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+      <c r="I19" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>30</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:29:35.558046</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5</v>
+      </c>
+      <c r="I20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>30</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:37:09.238480</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>15</v>
+      </c>
+      <c r="E21" t="n">
+        <v>15</v>
+      </c>
+      <c r="F21" t="n">
+        <v>15</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>15</v>
+      </c>
+      <c r="I21" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>40</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:39:48.093282</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>25</v>
+      </c>
+      <c r="E22" t="n">
+        <v>25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>25</v>
+      </c>
+      <c r="G22" t="n">
+        <v>21</v>
+      </c>
+      <c r="H22" t="n">
+        <v>25</v>
+      </c>
+      <c r="I22" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>40</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:41:46.891262</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>23</v>
+      </c>
+      <c r="E23" t="n">
+        <v>23</v>
+      </c>
+      <c r="F23" t="n">
+        <v>23</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" t="n">
+        <v>23</v>
+      </c>
+      <c r="I23" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>40</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:42:09.620661</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>12</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12</v>
+      </c>
+      <c r="G24" t="n">
+        <v>10</v>
+      </c>
+      <c r="H24" t="n">
+        <v>12</v>
+      </c>
+      <c r="I24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>40</v>
+      </c>
+      <c r="B25" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:43:02.467024</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>16</v>
+      </c>
+      <c r="E25" t="n">
+        <v>16</v>
+      </c>
+      <c r="F25" t="n">
+        <v>16</v>
+      </c>
+      <c r="G25" t="n">
+        <v>6</v>
+      </c>
+      <c r="H25" t="n">
+        <v>16</v>
+      </c>
+      <c r="I25" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>40</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:43:20.036084</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>20</v>
+      </c>
+      <c r="E26" t="n">
+        <v>20</v>
+      </c>
+      <c r="F26" t="n">
+        <v>20</v>
+      </c>
+      <c r="G26" t="n">
+        <v>8</v>
+      </c>
+      <c r="H26" t="n">
+        <v>20</v>
+      </c>
+      <c r="I26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>40</v>
+      </c>
+      <c r="B27" t="n">
+        <v>6</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:46:20.605873</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>8</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8</v>
+      </c>
+      <c r="I27" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>40</v>
+      </c>
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2021-04-08 13:54:29.560418</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>22</v>
+      </c>
+      <c r="E28" t="n">
+        <v>22</v>
+      </c>
+      <c r="F28" t="n">
+        <v>22</v>
+      </c>
+      <c r="G28" t="n">
+        <v>19</v>
+      </c>
+      <c r="H28" t="n">
+        <v>22</v>
+      </c>
+      <c r="I28" t="n">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit made to merge. synthetic graph driver implemented. Does not work at the moment (infinite loops)
</commit_message>
<xml_diff>
--- a/currently_in_use/tests/Test_results.xlsx
+++ b/currently_in_use/tests/Test_results.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -587,6 +587,189 @@
         <v>24</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>50</v>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2021-04-01 04:15:40.364422</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21</v>
+      </c>
+      <c r="H5" t="n">
+        <v>25</v>
+      </c>
+      <c r="I5" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2021-04-01 04:18:00.339001</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>19</v>
+      </c>
+      <c r="F6" t="n">
+        <v>19</v>
+      </c>
+      <c r="G6" t="n">
+        <v>18</v>
+      </c>
+      <c r="H6" t="n">
+        <v>19</v>
+      </c>
+      <c r="I6" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>50</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2021-04-01 04:20:35.999069</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>22</v>
+      </c>
+      <c r="E7" t="n">
+        <v>21</v>
+      </c>
+      <c r="F7" t="n">
+        <v>21</v>
+      </c>
+      <c r="G7" t="n">
+        <v>21</v>
+      </c>
+      <c r="H7" t="n">
+        <v>21</v>
+      </c>
+      <c r="I7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>50</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2021-04-01 04:31:17.323771</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>17</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" t="n">
+        <v>18</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2021-04-01 04:32:29.436554</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>27</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>26</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>26</v>
+      </c>
+      <c r="I9" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>50</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2021-04-04 04:51:56.682948</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
brute force using bipartite implemented. think works
</commit_message>
<xml_diff>
--- a/currently_in_use/tests/Test_results.xlsx
+++ b/currently_in_use/tests/Test_results.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -770,6 +770,440 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>30</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:16:00.140322</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>30</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:16:51.742843</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>30</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:46:32.245210</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>30</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:48:25.206486</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:50:16.661164</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7</v>
+      </c>
+      <c r="F15" t="n">
+        <v>7</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7</v>
+      </c>
+      <c r="I15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2021-04-14 23:54:28.575005</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:12:56.141677</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>9</v>
+      </c>
+      <c r="I17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>15</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:45:35.189974</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:46:01.736827</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>15</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:46:47.675392</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>15</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:48:23.374307</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" t="n">
+        <v>4</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>15</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2021-04-15 13:51:07.392178</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>15</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2021-04-15 14:10:51.898023</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>15</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2021-04-15 14:12:56.397366</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>3</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
major commit. Reworked graph creation so that cluster graph and bipartite graphs are created in the same file, based on original graph. Removed unused code. Created view class, which plots and records data and results of test files in same place. Made a new driver, which can take user input to create new test files or repeatadley test old test files. Promising repetition here. Every graph, and data used to create it, is saved (except bipartite graph, which will be implemented next (maybe?). Next goal is reorganization of folders etc within this repo. Several areas still need to update comments and standardize style.
</commit_message>
<xml_diff>
--- a/currently_in_use/tests/Test_results.xlsx
+++ b/currently_in_use/tests/Test_results.xlsx
@@ -501,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R693"/>
+  <dimension ref="A1:R709"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A633" ySplit="1"/>
@@ -48339,6 +48339,982 @@
         <v>9</v>
       </c>
     </row>
+    <row r="694">
+      <c r="A694" t="n">
+        <v>100</v>
+      </c>
+      <c r="B694" t="n">
+        <v>5</v>
+      </c>
+      <c r="C694" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:32.720444</t>
+        </is>
+      </c>
+      <c r="F694" t="n">
+        <v>4</v>
+      </c>
+      <c r="G694" t="n">
+        <v>2</v>
+      </c>
+      <c r="H694" t="n">
+        <v>2</v>
+      </c>
+      <c r="I694" t="n">
+        <v>2</v>
+      </c>
+      <c r="J694" t="n">
+        <v>15</v>
+      </c>
+      <c r="K694" t="n">
+        <v>15</v>
+      </c>
+      <c r="L694" t="n">
+        <v>15</v>
+      </c>
+      <c r="M694" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N694" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O694" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="n">
+        <v>100</v>
+      </c>
+      <c r="B695" t="n">
+        <v>5</v>
+      </c>
+      <c r="C695" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:34.256386</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L695" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M695" t="n">
+        <v>15</v>
+      </c>
+      <c r="N695" t="n">
+        <v>15</v>
+      </c>
+      <c r="O695" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="n">
+        <v>100</v>
+      </c>
+      <c r="B696" t="n">
+        <v>5</v>
+      </c>
+      <c r="C696" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:35.501490</t>
+        </is>
+      </c>
+      <c r="F696" t="n">
+        <v>8</v>
+      </c>
+      <c r="G696" t="n">
+        <v>9</v>
+      </c>
+      <c r="H696" t="n">
+        <v>9</v>
+      </c>
+      <c r="I696" t="n">
+        <v>9</v>
+      </c>
+      <c r="J696" t="n">
+        <v>10</v>
+      </c>
+      <c r="K696" t="n">
+        <v>10</v>
+      </c>
+      <c r="L696" t="n">
+        <v>10</v>
+      </c>
+      <c r="M696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="n">
+        <v>100</v>
+      </c>
+      <c r="B697" t="n">
+        <v>5</v>
+      </c>
+      <c r="C697" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:36.580797</t>
+        </is>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L697" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M697" t="n">
+        <v>10</v>
+      </c>
+      <c r="N697" t="n">
+        <v>10</v>
+      </c>
+      <c r="O697" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="n">
+        <v>100</v>
+      </c>
+      <c r="B698" t="n">
+        <v>5</v>
+      </c>
+      <c r="C698" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:37.738037</t>
+        </is>
+      </c>
+      <c r="F698" t="n">
+        <v>1</v>
+      </c>
+      <c r="G698" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H698" t="n">
+        <v>1</v>
+      </c>
+      <c r="I698" t="n">
+        <v>1</v>
+      </c>
+      <c r="J698" t="n">
+        <v>1</v>
+      </c>
+      <c r="K698" t="n">
+        <v>1</v>
+      </c>
+      <c r="L698" t="n">
+        <v>1</v>
+      </c>
+      <c r="M698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="n">
+        <v>100</v>
+      </c>
+      <c r="B699" t="n">
+        <v>5</v>
+      </c>
+      <c r="C699" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:39.095243</t>
+        </is>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L699" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M699" t="n">
+        <v>1</v>
+      </c>
+      <c r="N699" t="n">
+        <v>1</v>
+      </c>
+      <c r="O699" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="n">
+        <v>100</v>
+      </c>
+      <c r="B700" t="n">
+        <v>5</v>
+      </c>
+      <c r="C700" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:40.352415</t>
+        </is>
+      </c>
+      <c r="F700" t="n">
+        <v>14</v>
+      </c>
+      <c r="G700" t="n">
+        <v>14</v>
+      </c>
+      <c r="H700" t="n">
+        <v>11</v>
+      </c>
+      <c r="I700" t="n">
+        <v>14</v>
+      </c>
+      <c r="J700" t="n">
+        <v>14</v>
+      </c>
+      <c r="K700" t="n">
+        <v>14</v>
+      </c>
+      <c r="L700" t="n">
+        <v>14</v>
+      </c>
+      <c r="M700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="n">
+        <v>100</v>
+      </c>
+      <c r="B701" t="n">
+        <v>5</v>
+      </c>
+      <c r="C701" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:41.731323</t>
+        </is>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L701" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M701" t="n">
+        <v>13</v>
+      </c>
+      <c r="N701" t="n">
+        <v>13</v>
+      </c>
+      <c r="O701" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="n">
+        <v>100</v>
+      </c>
+      <c r="B702" t="n">
+        <v>5</v>
+      </c>
+      <c r="C702" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:15.167025</t>
+        </is>
+      </c>
+      <c r="F702" t="n">
+        <v>16</v>
+      </c>
+      <c r="G702" t="n">
+        <v>14</v>
+      </c>
+      <c r="H702" t="n">
+        <v>14</v>
+      </c>
+      <c r="I702" t="n">
+        <v>14</v>
+      </c>
+      <c r="J702" t="n">
+        <v>14</v>
+      </c>
+      <c r="K702" t="n">
+        <v>14</v>
+      </c>
+      <c r="L702" t="n">
+        <v>14</v>
+      </c>
+      <c r="M702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="n">
+        <v>100</v>
+      </c>
+      <c r="B703" t="n">
+        <v>5</v>
+      </c>
+      <c r="C703" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:16.363163</t>
+        </is>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L703" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M703" t="n">
+        <v>14</v>
+      </c>
+      <c r="N703" t="n">
+        <v>14</v>
+      </c>
+      <c r="O703" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="n">
+        <v>100</v>
+      </c>
+      <c r="B704" t="n">
+        <v>5</v>
+      </c>
+      <c r="C704" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:17.438332</t>
+        </is>
+      </c>
+      <c r="F704" t="n">
+        <v>3</v>
+      </c>
+      <c r="G704" t="n">
+        <v>-11</v>
+      </c>
+      <c r="H704" t="n">
+        <v>0</v>
+      </c>
+      <c r="I704" t="n">
+        <v>1</v>
+      </c>
+      <c r="J704" t="n">
+        <v>1</v>
+      </c>
+      <c r="K704" t="n">
+        <v>1</v>
+      </c>
+      <c r="L704" t="n">
+        <v>-2</v>
+      </c>
+      <c r="M704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="n">
+        <v>100</v>
+      </c>
+      <c r="B705" t="n">
+        <v>5</v>
+      </c>
+      <c r="C705" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:18.664559</t>
+        </is>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L705" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M705" t="n">
+        <v>1</v>
+      </c>
+      <c r="N705" t="n">
+        <v>1</v>
+      </c>
+      <c r="O705" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="n">
+        <v>100</v>
+      </c>
+      <c r="B706" t="n">
+        <v>5</v>
+      </c>
+      <c r="C706" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:19.916148</t>
+        </is>
+      </c>
+      <c r="F706" t="n">
+        <v>4</v>
+      </c>
+      <c r="G706" t="n">
+        <v>2</v>
+      </c>
+      <c r="H706" t="n">
+        <v>2</v>
+      </c>
+      <c r="I706" t="n">
+        <v>2</v>
+      </c>
+      <c r="J706" t="n">
+        <v>3</v>
+      </c>
+      <c r="K706" t="n">
+        <v>0</v>
+      </c>
+      <c r="L706" t="n">
+        <v>3</v>
+      </c>
+      <c r="M706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>100</v>
+      </c>
+      <c r="B707" t="n">
+        <v>5</v>
+      </c>
+      <c r="C707" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:21.013486</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L707" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M707" t="n">
+        <v>3</v>
+      </c>
+      <c r="N707" t="n">
+        <v>0</v>
+      </c>
+      <c r="O707" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>100</v>
+      </c>
+      <c r="B708" t="n">
+        <v>5</v>
+      </c>
+      <c r="C708" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:22.083597</t>
+        </is>
+      </c>
+      <c r="F708" t="n">
+        <v>14</v>
+      </c>
+      <c r="G708" t="n">
+        <v>12</v>
+      </c>
+      <c r="H708" t="n">
+        <v>13</v>
+      </c>
+      <c r="I708" t="n">
+        <v>14</v>
+      </c>
+      <c r="J708" t="n">
+        <v>14</v>
+      </c>
+      <c r="K708" t="n">
+        <v>14</v>
+      </c>
+      <c r="L708" t="n">
+        <v>13</v>
+      </c>
+      <c r="M708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="n">
+        <v>100</v>
+      </c>
+      <c r="B709" t="n">
+        <v>5</v>
+      </c>
+      <c r="C709" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:23.418709</t>
+        </is>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L709" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M709" t="n">
+        <v>4</v>
+      </c>
+      <c r="N709" t="n">
+        <v>3</v>
+      </c>
+      <c r="O709" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:Q1048576 R89:R677">
     <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
@@ -48358,7 +49334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L694"/>
+  <dimension ref="A1:L710"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A599" ySplit="1"/>
@@ -80320,6 +81296,742 @@
         <v>0.01359309999999958</v>
       </c>
     </row>
+    <row r="695">
+      <c r="A695" t="n">
+        <v>100</v>
+      </c>
+      <c r="B695" t="n">
+        <v>5</v>
+      </c>
+      <c r="C695" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:32.720444</t>
+        </is>
+      </c>
+      <c r="F695" t="n">
+        <v>0.04976590000000058</v>
+      </c>
+      <c r="G695" t="n">
+        <v>5.920000000081416e-05</v>
+      </c>
+      <c r="H695" t="n">
+        <v>0.04490209999999983</v>
+      </c>
+      <c r="I695" t="n">
+        <v>0.1264978000000001</v>
+      </c>
+      <c r="J695" t="n">
+        <v>0.03520579999999995</v>
+      </c>
+      <c r="K695" t="n">
+        <v>0.001519000000000048</v>
+      </c>
+      <c r="L695" t="n">
+        <v>0.004674200000000184</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="n">
+        <v>100</v>
+      </c>
+      <c r="B696" t="n">
+        <v>5</v>
+      </c>
+      <c r="C696" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:34.256386</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I696" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J696" t="n">
+        <v>0.03518600000000038</v>
+      </c>
+      <c r="K696" t="n">
+        <v>0.0020876000000003</v>
+      </c>
+      <c r="L696" t="n">
+        <v>0.005920099999999984</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="n">
+        <v>100</v>
+      </c>
+      <c r="B697" t="n">
+        <v>5</v>
+      </c>
+      <c r="C697" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:35.501490</t>
+        </is>
+      </c>
+      <c r="F697" t="n">
+        <v>0.01122630000000058</v>
+      </c>
+      <c r="G697" t="n">
+        <v>4.139999999885902e-05</v>
+      </c>
+      <c r="H697" t="n">
+        <v>0.004135199999998562</v>
+      </c>
+      <c r="I697" t="n">
+        <v>0.02822910000000078</v>
+      </c>
+      <c r="J697" t="n">
+        <v>0.02811479999999911</v>
+      </c>
+      <c r="K697" t="n">
+        <v>0.0009005999999995851</v>
+      </c>
+      <c r="L697" t="n">
+        <v>0.002771700000000266</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="n">
+        <v>100</v>
+      </c>
+      <c r="B698" t="n">
+        <v>5</v>
+      </c>
+      <c r="C698" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:36.580797</t>
+        </is>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I698" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J698" t="n">
+        <v>0.02917229999999904</v>
+      </c>
+      <c r="K698" t="n">
+        <v>0.001201599999999914</v>
+      </c>
+      <c r="L698" t="n">
+        <v>0.003455799999999343</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="n">
+        <v>100</v>
+      </c>
+      <c r="B699" t="n">
+        <v>5</v>
+      </c>
+      <c r="C699" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:37.738037</t>
+        </is>
+      </c>
+      <c r="F699" t="n">
+        <v>0.001196900000000056</v>
+      </c>
+      <c r="G699" t="n">
+        <v>7.62999999999181e-05</v>
+      </c>
+      <c r="H699" t="n">
+        <v>0.0008893000000007589</v>
+      </c>
+      <c r="I699" t="n">
+        <v>0.02579710000000013</v>
+      </c>
+      <c r="J699" t="n">
+        <v>0.02974460000000079</v>
+      </c>
+      <c r="K699" t="n">
+        <v>0.002602300000001279</v>
+      </c>
+      <c r="L699" t="n">
+        <v>0.004880999999999247</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="n">
+        <v>100</v>
+      </c>
+      <c r="B700" t="n">
+        <v>5</v>
+      </c>
+      <c r="C700" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:39.095243</t>
+        </is>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I700" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J700" t="n">
+        <v>0.02962920000000047</v>
+      </c>
+      <c r="K700" t="n">
+        <v>0.002230700000000141</v>
+      </c>
+      <c r="L700" t="n">
+        <v>0.00433679999999903</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="n">
+        <v>100</v>
+      </c>
+      <c r="B701" t="n">
+        <v>5</v>
+      </c>
+      <c r="C701" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:40.352415</t>
+        </is>
+      </c>
+      <c r="F701" t="n">
+        <v>0.001701599999998749</v>
+      </c>
+      <c r="G701" t="n">
+        <v>6.899999999987472e-05</v>
+      </c>
+      <c r="H701" t="n">
+        <v>0.01722519999999861</v>
+      </c>
+      <c r="I701" t="n">
+        <v>0.03470490000000126</v>
+      </c>
+      <c r="J701" t="n">
+        <v>0.03040220000000105</v>
+      </c>
+      <c r="K701" t="n">
+        <v>0.001623300000000327</v>
+      </c>
+      <c r="L701" t="n">
+        <v>0.005242399999998426</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="n">
+        <v>100</v>
+      </c>
+      <c r="B702" t="n">
+        <v>5</v>
+      </c>
+      <c r="C702" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:37:41.731323</t>
+        </is>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I702" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J702" t="n">
+        <v>0.03181549999999866</v>
+      </c>
+      <c r="K702" t="n">
+        <v>0.001281900000000391</v>
+      </c>
+      <c r="L702" t="n">
+        <v>0.004743299999999451</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="n">
+        <v>100</v>
+      </c>
+      <c r="B703" t="n">
+        <v>5</v>
+      </c>
+      <c r="C703" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>ba-no-cycle</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:15.167025</t>
+        </is>
+      </c>
+      <c r="F703" t="n">
+        <v>0.001415399999999956</v>
+      </c>
+      <c r="G703" t="n">
+        <v>4.319999999990998e-05</v>
+      </c>
+      <c r="H703" t="n">
+        <v>0.0006435000000002411</v>
+      </c>
+      <c r="I703" t="n">
+        <v>0.03166400000000014</v>
+      </c>
+      <c r="J703" t="n">
+        <v>0.03287930000000028</v>
+      </c>
+      <c r="K703" t="n">
+        <v>0.00128869999999992</v>
+      </c>
+      <c r="L703" t="n">
+        <v>0.003823500000000202</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="n">
+        <v>100</v>
+      </c>
+      <c r="B704" t="n">
+        <v>5</v>
+      </c>
+      <c r="C704" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>ba-cycle</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:16.363163</t>
+        </is>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I704" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J704" t="n">
+        <v>0.0306002000000003</v>
+      </c>
+      <c r="K704" t="n">
+        <v>0.001087700000000247</v>
+      </c>
+      <c r="L704" t="n">
+        <v>0.003167200000000037</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="n">
+        <v>100</v>
+      </c>
+      <c r="B705" t="n">
+        <v>5</v>
+      </c>
+      <c r="C705" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>er-no-cycle</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:17.438332</t>
+        </is>
+      </c>
+      <c r="F705" t="n">
+        <v>0.001273200000000863</v>
+      </c>
+      <c r="G705" t="n">
+        <v>4.739999999969768e-05</v>
+      </c>
+      <c r="H705" t="n">
+        <v>0.04664279999999987</v>
+      </c>
+      <c r="I705" t="n">
+        <v>0.03127879999999994</v>
+      </c>
+      <c r="J705" t="n">
+        <v>0.05611419999999967</v>
+      </c>
+      <c r="K705" t="n">
+        <v>0.002721799999999774</v>
+      </c>
+      <c r="L705" t="n">
+        <v>0.00522530000000021</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="n">
+        <v>100</v>
+      </c>
+      <c r="B706" t="n">
+        <v>5</v>
+      </c>
+      <c r="C706" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>er-cycle</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:18.664559</t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I706" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J706" t="n">
+        <v>0.05648840000000011</v>
+      </c>
+      <c r="K706" t="n">
+        <v>0.002850500000000089</v>
+      </c>
+      <c r="L706" t="n">
+        <v>0.006328499999999515</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>100</v>
+      </c>
+      <c r="B707" t="n">
+        <v>5</v>
+      </c>
+      <c r="C707" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>ws-no-cycle</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:19.916148</t>
+        </is>
+      </c>
+      <c r="F707" t="n">
+        <v>0.0006739000000006712</v>
+      </c>
+      <c r="G707" t="n">
+        <v>2.939999999895804e-05</v>
+      </c>
+      <c r="H707" t="n">
+        <v>0.0002706000000003428</v>
+      </c>
+      <c r="I707" t="n">
+        <v>0.02959759999999889</v>
+      </c>
+      <c r="J707" t="n">
+        <v>0.03197600000000023</v>
+      </c>
+      <c r="K707" t="n">
+        <v>0.001204300000001268</v>
+      </c>
+      <c r="L707" t="n">
+        <v>0.003281199999999984</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>100</v>
+      </c>
+      <c r="B708" t="n">
+        <v>5</v>
+      </c>
+      <c r="C708" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>ws-cycle</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:21.013486</t>
+        </is>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I708" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J708" t="n">
+        <v>0.03321019999999919</v>
+      </c>
+      <c r="K708" t="n">
+        <v>0.001198799999999167</v>
+      </c>
+      <c r="L708" t="n">
+        <v>0.002681400000000167</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="n">
+        <v>100</v>
+      </c>
+      <c r="B709" t="n">
+        <v>5</v>
+      </c>
+      <c r="C709" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>cluster no cycle</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:22.083597</t>
+        </is>
+      </c>
+      <c r="F709" t="n">
+        <v>0.00184530000000116</v>
+      </c>
+      <c r="G709" t="n">
+        <v>5.100000000091143e-05</v>
+      </c>
+      <c r="H709" t="n">
+        <v>0.01588459999999969</v>
+      </c>
+      <c r="I709" t="n">
+        <v>0.03523429999999905</v>
+      </c>
+      <c r="J709" t="n">
+        <v>0.03513260000000074</v>
+      </c>
+      <c r="K709" t="n">
+        <v>0.002214999999999634</v>
+      </c>
+      <c r="L709" t="n">
+        <v>0.008323600000000653</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="n">
+        <v>100</v>
+      </c>
+      <c r="B710" t="n">
+        <v>5</v>
+      </c>
+      <c r="C710" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>cluster cycle</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>2021-06-17 11:38:23.418709</t>
+        </is>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I710" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J710" t="n">
+        <v>0.0340246999999998</v>
+      </c>
+      <c r="K710" t="n">
+        <v>0.002088699999999832</v>
+      </c>
+      <c r="L710" t="n">
+        <v>0.007329300000000316</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>